<commit_message>
Started figuring out how to measure biodiversity of sites
</commit_message>
<xml_diff>
--- a/vesDataMaster.xlsx
+++ b/vesDataMaster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepos\VTADS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DE0281-84D6-48DB-B528-F0E02A4CCE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2861AC6B-D657-479B-9E3C-B51BDC43CA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{54C3C1A8-21CD-4FD0-B5D4-BFED4F1CBA7A}"/>
   </bookViews>
@@ -1252,7 +1252,7 @@
   <dimension ref="A1:Y1806"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1664" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A1602" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B1728" sqref="B1728:B1730"/>
     </sheetView>
   </sheetViews>
@@ -62001,7 +62001,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1602" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1602" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1602" s="1" t="s">
         <v>74</v>
       </c>
@@ -62544,7 +62544,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1617" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1617" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1617" s="1" t="s">
         <v>74</v>
       </c>
@@ -63531,7 +63531,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1650" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1650" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1650" s="1" t="s">
         <v>74</v>
       </c>
@@ -63567,7 +63567,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1651" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1651" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1651" s="1" t="s">
         <v>74</v>
       </c>
@@ -63606,7 +63606,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="1652" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1652" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1652" s="1" t="s">
         <v>74</v>
       </c>
@@ -63642,7 +63642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1653" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1653" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1653" s="1" t="s">
         <v>74</v>
       </c>
@@ -63678,7 +63678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1654" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1654" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1654" s="1" t="s">
         <v>74</v>
       </c>
@@ -63714,7 +63714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="1655" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1655" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1655" s="1" t="s">
         <v>74</v>
       </c>
@@ -64038,7 +64038,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1664" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1664" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1664" s="1" t="s">
         <v>84</v>
       </c>
@@ -64074,7 +64074,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1665" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1665" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1665" s="1" t="s">
         <v>84</v>
       </c>
@@ -64110,7 +64110,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1666" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1666" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1666" s="1" t="s">
         <v>84</v>
       </c>
@@ -66096,7 +66096,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1721" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1721" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1721" s="1" t="s">
         <v>84</v>
       </c>
@@ -66132,7 +66132,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1722" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1722" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1722" s="1" t="s">
         <v>84</v>
       </c>
@@ -66168,7 +66168,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1723" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1723" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1723" s="1" t="s">
         <v>84</v>
       </c>
@@ -66204,7 +66204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1724" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1724" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1724" s="1" t="s">
         <v>84</v>
       </c>
@@ -66240,7 +66240,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="1725" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1725" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1725" s="1" t="s">
         <v>84</v>
       </c>
@@ -66276,7 +66276,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1726" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1726" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1726" s="1" t="s">
         <v>84</v>
       </c>
@@ -66315,7 +66315,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="1727" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1727" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1727" s="1" t="s">
         <v>84</v>
       </c>
@@ -66351,7 +66351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1728" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1728" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1728" s="1" t="s">
         <v>84</v>
       </c>
@@ -66387,7 +66387,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1729" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1729" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1729" s="1" t="s">
         <v>84</v>
       </c>
@@ -66423,7 +66423,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="1730" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1730" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1730" s="1" t="s">
         <v>84</v>
       </c>
@@ -68107,7 +68107,7 @@
   <autoFilter ref="A1:O1772" xr:uid="{3A70FAE1-061C-4903-859C-F71BE94E0541}">
     <filterColumn colId="2">
       <filters>
-        <filter val="12-3"/>
+        <filter val="09-01"/>
       </filters>
     </filterColumn>
     <filterColumn colId="4">
@@ -68385,26 +68385,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="94106a43-364c-4431-a764-9e3dd608a139" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f61aad6-7023-4354-b4be-ac6efb5d4555">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D153441376FC57458463DD41A74D2A65" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a4326ad5c94cf01f5c89c634265e4dfe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f61aad6-7023-4354-b4be-ac6efb5d4555" xmlns:ns3="94106a43-364c-4431-a764-9e3dd608a139" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d131896e5ee02cd0fe36e0cf600b076" ns2:_="" ns3:_="">
     <xsd:import namespace="6f61aad6-7023-4354-b4be-ac6efb5d4555"/>
@@ -68637,10 +68617,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="94106a43-364c-4431-a764-9e3dd608a139" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f61aad6-7023-4354-b4be-ac6efb5d4555">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B28517-83EC-425D-ACE8-0BB7EF9CCA9D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30AE564B-B026-4F92-B372-9EB3FE3A62D1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6f61aad6-7023-4354-b4be-ac6efb5d4555"/>
+    <ds:schemaRef ds:uri="94106a43-364c-4431-a764-9e3dd608a139"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -68657,20 +68668,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30AE564B-B026-4F92-B372-9EB3FE3A62D1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3B28517-83EC-425D-ACE8-0BB7EF9CCA9D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6f61aad6-7023-4354-b4be-ac6efb5d4555"/>
-    <ds:schemaRef ds:uri="94106a43-364c-4431-a764-9e3dd608a139"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>